<commit_message>
[IMP] import_account_opening: Parter account from Excel file /Conto cliente/fornitore da file Excel
</commit_message>
<xml_diff>
--- a/import_account_opening/example/example.xlsx
+++ b/import_account_opening/example/example.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t xml:space="preserve">Codice</t>
   </si>
@@ -37,22 +37,40 @@
     <t xml:space="preserve">Partita IVA</t>
   </si>
   <si>
+    <t xml:space="preserve">Ref</t>
+  </si>
+  <si>
     <t xml:space="preserve">Dare</t>
   </si>
   <si>
     <t xml:space="preserve">Avere</t>
   </si>
   <si>
-    <t xml:space="preserve">Global Trading Ltd</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GB250072348000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rossi e Bianchi srl</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IT05111810015</t>
+    <t xml:space="preserve">Prima Alpha S.p.A.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IT00115719999</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Notaio Decimo Jackson</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IT10242670015</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Latte Beta Due s.n.c.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IT02345670018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RiBA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Freie Universität Berlin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DE123456788</t>
   </si>
   <si>
     <t xml:space="preserve">Banca</t>
@@ -152,15 +170,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="29.08"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="8.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10.97"/>
@@ -189,43 +207,80 @@
       <c r="G1" s="0" t="s">
         <v>6</v>
       </c>
+      <c r="H1" s="0" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>1</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="G2" s="0" t="n">
         <v>1000</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D3" s="0" t="n">
         <v>1</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="G3" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="H3" s="0" t="n">
         <v>500</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
+        <v>152220</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" s="0" t="n">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5" s="0" t="n">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
         <v>180003</v>
       </c>
-      <c r="B4" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" s="0" t="n">
+      <c r="B6" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6" s="0" t="n">
         <v>100</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[IMP] import_account_opening: new features
</commit_message>
<xml_diff>
--- a/import_account_opening/example/example.xlsx
+++ b/import_account_opening/example/example.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
   <si>
     <t xml:space="preserve">Codice</t>
   </si>
@@ -70,7 +70,10 @@
     <t xml:space="preserve">Freie Universität Berlin</t>
   </si>
   <si>
-    <t xml:space="preserve">DE123456788</t>
+    <t xml:space="preserve">Mario Rossi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RSSMRA69C02D612M</t>
   </si>
   <si>
     <t xml:space="preserve">Banca</t>
@@ -170,19 +173,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+      <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="29.08"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="8.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10.97"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="15.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="19.45"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -227,60 +230,85 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="H3" s="0" t="n">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E3" s="0" t="s">
+      <c r="D4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E4" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="H3" s="0" t="n">
+      <c r="H4" s="0" t="n">
         <v>500</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
         <v>152220</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B5" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E4" s="0" t="s">
+      <c r="C5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E5" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="0" t="s">
+      <c r="F5" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="0" t="n">
+      <c r="G5" s="0" t="n">
         <v>150</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="0" t="s">
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E5" s="0" t="s">
+      <c r="D6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H6" s="0" t="n">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="H5" s="0" t="n">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="n">
+      <c r="C7" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="G7" s="0" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="n">
         <v>180003</v>
       </c>
-      <c r="B6" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="G6" s="0" t="n">
+      <c r="B8" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="G8" s="0" t="n">
         <v>100</v>
       </c>
     </row>

</xml_diff>